<commit_message>
Intento corregir el tim0
</commit_message>
<xml_diff>
--- a/ProyectoEstacion/Memoria/Rubricas.xlsx
+++ b/ProyectoEstacion/Memoria/Rubricas.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DFBF5E-B2A5-4116-909B-ACEAEC05DDA0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -136,7 +135,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -510,11 +509,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +571,7 @@
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="8"/>
+      <c r="G6" s="9"/>
       <c r="H6" s="8"/>
       <c r="I6" t="s">
         <v>28</v>
@@ -727,7 +726,7 @@
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
-      <c r="H19" s="8"/>
+      <c r="H19" s="9"/>
       <c r="I19" t="s">
         <v>33</v>
       </c>

</xml_diff>